<commit_message>
Fixing field slots bug
</commit_message>
<xml_diff>
--- a/data/Пожелания.xlsx
+++ b/data/Пожелания.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>ID</t>
   </si>
@@ -26,36 +26,6 @@
   </si>
   <si>
     <t>по</t>
-  </si>
-  <si>
-    <t>09:00</t>
-  </si>
-  <si>
-    <t>17:30</t>
-  </si>
-  <si>
-    <t>15:00</t>
-  </si>
-  <si>
-    <t>23:00</t>
-  </si>
-  <si>
-    <t>16:00</t>
-  </si>
-  <si>
-    <t>17:00</t>
-  </si>
-  <si>
-    <t>12:00</t>
-  </si>
-  <si>
-    <t>13:00</t>
-  </si>
-  <si>
-    <t>12</t>
-  </si>
-  <si>
-    <t>63</t>
   </si>
 </sst>
 </file>
@@ -379,174 +349,6 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
-      <c r="C2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3">
-        <v>2</v>
-      </c>
-      <c r="C3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4">
-        <v>19</v>
-      </c>
-      <c r="C4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5">
-        <v>20</v>
-      </c>
-      <c r="C5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6">
-        <v>25</v>
-      </c>
-      <c r="C6" t="s">
-        <v>6</v>
-      </c>
-      <c r="D6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7">
-        <v>6</v>
-      </c>
-      <c r="B7">
-        <v>26</v>
-      </c>
-      <c r="C7" t="s">
-        <v>8</v>
-      </c>
-      <c r="D7" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8">
-        <v>7</v>
-      </c>
-      <c r="B8">
-        <v>31</v>
-      </c>
-      <c r="C8" t="s">
-        <v>4</v>
-      </c>
-      <c r="D8" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9">
-        <v>8</v>
-      </c>
-      <c r="B9">
-        <v>32</v>
-      </c>
-      <c r="C9" t="s">
-        <v>4</v>
-      </c>
-      <c r="D9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10">
-        <v>9</v>
-      </c>
-      <c r="B10">
-        <v>42</v>
-      </c>
-      <c r="C10" t="s">
-        <v>10</v>
-      </c>
-      <c r="D10" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11">
-        <v>10</v>
-      </c>
-      <c r="B11">
-        <v>54</v>
-      </c>
-      <c r="C11" t="s">
-        <v>6</v>
-      </c>
-      <c r="D11" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12">
-        <v>11</v>
-      </c>
-      <c r="B12">
-        <v>62</v>
-      </c>
-      <c r="C12" t="s">
-        <v>11</v>
-      </c>
-      <c r="D12" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="s">
-        <v>12</v>
-      </c>
-      <c r="B13" t="s">
-        <v>13</v>
-      </c>
-      <c r="C13" t="s">
-        <v>4</v>
-      </c>
-      <c r="D13" t="s">
-        <v>8</v>
-      </c>
-    </row>
   </sheetData>
 </worksheet>
 </file>
</xml_diff>